<commit_message>
added KPD, MHM, OHS, OST
</commit_message>
<xml_diff>
--- a/cello_to_onco_mapping_final.xlsx
+++ b/cello_to_onco_mapping_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sisira/Google Drive/BHKLab/Oncotree mapping/myMapping/DataCuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sisira/Desktop/Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423B205-3459-F14E-919C-01A554A16B75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E97731-484D-F540-99B6-6377CF64EE76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="460" windowWidth="33900" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13060" yWindow="1580" windowWidth="33900" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cello_to_onco_mapping_1_all" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22294" uniqueCount="5650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22346" uniqueCount="5658">
   <si>
     <t>unique.cellid</t>
   </si>
@@ -16973,6 +16973,30 @@
   </si>
   <si>
     <t>cellosaurus name</t>
+  </si>
+  <si>
+    <t>KPD</t>
+  </si>
+  <si>
+    <t>CVCL_B412</t>
+  </si>
+  <si>
+    <t>CVCL_B426</t>
+  </si>
+  <si>
+    <t>MHM</t>
+  </si>
+  <si>
+    <t>CVCL_B450</t>
+  </si>
+  <si>
+    <t>OHS</t>
+  </si>
+  <si>
+    <t>CVCL_8399</t>
+  </si>
+  <si>
+    <t>OST</t>
   </si>
 </sst>
 </file>
@@ -17821,11 +17845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1715"/>
+  <dimension ref="A1:O1719"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <pane ySplit="1" topLeftCell="A1696" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1710" sqref="C1710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -93316,6 +93340,182 @@
         <v>121</v>
       </c>
     </row>
+    <row r="1716" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1716">
+        <v>1719</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>5650</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>5650</v>
+      </c>
+      <c r="D1716" t="s">
+        <v>5651</v>
+      </c>
+      <c r="E1716" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1716" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1716" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1716" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1716" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1716" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1716" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1716" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1716" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1716" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1717">
+        <v>1720</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>5653</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>5653</v>
+      </c>
+      <c r="D1717" t="s">
+        <v>5652</v>
+      </c>
+      <c r="E1717" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1717" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1717" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1717" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1717" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1717" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1717" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1717" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1717" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1717" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1718">
+        <v>1721</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>5655</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>5655</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>5654</v>
+      </c>
+      <c r="E1718" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1718" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1718" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1718" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1718" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1718" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1718" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1718" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1718" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1718" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1719">
+        <v>1722</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>5657</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>5657</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>5656</v>
+      </c>
+      <c r="E1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1719" t="s">
+        <v>415</v>
+      </c>
+      <c r="G1719" t="s">
+        <v>416</v>
+      </c>
+      <c r="H1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1719" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1719" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>